<commit_message>
Added metier codes agreed in ISSG Metier on 20240304
</commit_message>
<xml_diff>
--- a/Metiers/Reference_lists/RDB_ISSG_Metier_level_7_list.xlsx
+++ b/Metiers/Reference_lists/RDB_ISSG_Metier_level_7_list.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\joeg\Metier work\RCG_intersessional_work_2023\Task1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JOEG\GitHub\RCGs\Metiers\Reference_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B90FBD2-874D-47D4-957E-00ED33B13896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32355" yWindow="3555" windowWidth="17280" windowHeight="11490" xr2:uid="{7A17986C-306E-42A9-BB84-4ECF9C19F924}"/>
+    <workbookView xWindow="32352" yWindow="3552" windowWidth="17280" windowHeight="11496"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$46</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="58">
   <si>
     <t>Metier_level7</t>
   </si>
@@ -204,12 +203,21 @@
   </si>
   <si>
     <t>LHP_LPF_0_0_0_SWO</t>
+  </si>
+  <si>
+    <t>LLS_LPF</t>
+  </si>
+  <si>
+    <t>LLS_LPF_0_0_0</t>
+  </si>
+  <si>
+    <t>LLS_LPF_0_0_0_SWP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -225,7 +233,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,6 +276,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -281,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -305,6 +319,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,11 +634,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1FD52D3-6B22-4C70-838B-6CE8FBF5413A}">
-  <dimension ref="A1:F45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1295,28 +1311,28 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F34">
-        <v>20230127</v>
+      <c r="A34" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="F34" s="17">
+        <v>20240311</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B35" s="12" t="s">
         <v>15</v>
@@ -1336,7 +1352,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B36" s="12" t="s">
         <v>15</v>
@@ -1356,7 +1372,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>15</v>
@@ -1375,20 +1391,20 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>51</v>
+      <c r="A38" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="F38">
         <v>20230127</v>
@@ -1399,10 +1415,10 @@
         <v>31</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D39" s="13" t="s">
         <v>41</v>
@@ -1419,10 +1435,10 @@
         <v>31</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D40" s="13" t="s">
         <v>41</v>
@@ -1439,10 +1455,10 @@
         <v>31</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D41" s="13" t="s">
         <v>41</v>
@@ -1458,11 +1474,11 @@
       <c r="A42" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="15" t="s">
-        <v>20</v>
+      <c r="B42" s="14" t="s">
+        <v>19</v>
       </c>
       <c r="C42" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D42" s="13" t="s">
         <v>41</v>
@@ -1475,20 +1491,20 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" s="5" t="s">
+      <c r="A43" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B43" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="E43" s="1" t="s">
-        <v>48</v>
+      <c r="E43" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="F43">
         <v>20230127</v>
@@ -1499,10 +1515,10 @@
         <v>32</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D44" s="5" t="s">
         <v>41</v>
@@ -1518,11 +1534,11 @@
       <c r="A45" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>23</v>
+      <c r="B45" s="16" t="s">
+        <v>22</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D45" s="5" t="s">
         <v>41</v>
@@ -1534,8 +1550,28 @@
         <v>20230127</v>
       </c>
     </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F46">
+        <v>20230127</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F45" xr:uid="{B1FD52D3-6B22-4C70-838B-6CE8FBF5413A}"/>
+  <autoFilter ref="A1:F46"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated with agreed metier codes Feb 2025
</commit_message>
<xml_diff>
--- a/Metiers/Reference_lists/RDB_ISSG_Metier_level_7_list.xlsx
+++ b/Metiers/Reference_lists/RDB_ISSG_Metier_level_7_list.xlsx
@@ -1,44 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\JOEG\GitHub\RCGs\Metiers\Reference_lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Q:\dfad\users\joeg\home\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB27A5D-90DB-4049-B066-640403B66DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32352" yWindow="3552" windowWidth="17280" windowHeight="11496"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DCF level7 metier ref list" sheetId="1" r:id="rId1"/>
+    <sheet name="School type - FADs codification" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'DCF level7 metier ref list'!$A$1:$F$46</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="122">
   <si>
     <t>Metier_level7</t>
   </si>
@@ -212,13 +203,205 @@
   </si>
   <si>
     <t>LLS_LPF_0_0_0_SWO</t>
+  </si>
+  <si>
+    <t>GNS_DEF_&gt;=220_0_0_LUM</t>
+  </si>
+  <si>
+    <t>GNS_DEF_&gt;=220_0_0</t>
+  </si>
+  <si>
+    <t>GNS_DEF</t>
+  </si>
+  <si>
+    <t>Lumpfish(=Lumpsuker) (Cyclopterus lumpus)</t>
+  </si>
+  <si>
+    <t>GNS_DEF_&gt;=220_0_0_COD</t>
+  </si>
+  <si>
+    <t>Atlantic cod (Gadus morhua)</t>
+  </si>
+  <si>
+    <t>LHM_LPF_0_0_0_BFT_AF</t>
+  </si>
+  <si>
+    <t>LHM_LPF_0_0_0_BFT_DF</t>
+  </si>
+  <si>
+    <t>LHM_LPF_0_0_0_BFT_FS</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_ALB_AF</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_ALB_DF</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_ALB_FS</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_BFT_AF</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_BFT_DF</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_BFT_FS</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_MSP_AF</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_MSP_DF</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_MSP_FS</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_SWO_AF</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_SWO_DF</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_SWO_FS</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_TRO_AF</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_TRO_DF</t>
+  </si>
+  <si>
+    <t>LHP_LPF_0_0_0_TRO_FS</t>
+  </si>
+  <si>
+    <t>LLD_LPF_0_0_0_ALB_AF</t>
+  </si>
+  <si>
+    <t>LLD_LPF_0_0_0_ALB_DF</t>
+  </si>
+  <si>
+    <t>LLD_LPF_0_0_0_ALB_FS</t>
+  </si>
+  <si>
+    <t>LLD_LPF_0_0_0_BFT_AF</t>
+  </si>
+  <si>
+    <t>LLD_LPF_0_0_0_BFT_DF</t>
+  </si>
+  <si>
+    <t>LLD_LPF_0_0_0_BFT_FS</t>
+  </si>
+  <si>
+    <t>LLD_LPF_0_0_0_SWO_AF</t>
+  </si>
+  <si>
+    <t>LLD_LPF_0_0_0_SWO_DF</t>
+  </si>
+  <si>
+    <t>LLD_LPF_0_0_0_SWO_FS</t>
+  </si>
+  <si>
+    <t>LTL_LPF_0_0_0_ALB_AF</t>
+  </si>
+  <si>
+    <t>LTL_LPF_0_0_0_ALB_DF</t>
+  </si>
+  <si>
+    <t>LTL_LPF_0_0_0_ALB_FS</t>
+  </si>
+  <si>
+    <t>PS_LPF_&gt;=120_0_0_TRO_AF</t>
+  </si>
+  <si>
+    <t>PS_LPF_&gt;=120_0_0_TRO_DF</t>
+  </si>
+  <si>
+    <t>PS_LPF_&gt;=120_0_0_TRO_FS</t>
+  </si>
+  <si>
+    <t>PS_LPF_&gt;0_0_0_TRO_AF</t>
+  </si>
+  <si>
+    <t>PS_LPF_&gt;0_0_0_TRO_DF</t>
+  </si>
+  <si>
+    <t>PS_LPF_&gt;0_0_0_TRO_FS</t>
+  </si>
+  <si>
+    <t>PS_LPF_10-31_0_0_TRO_AF</t>
+  </si>
+  <si>
+    <t>PS_LPF_10-31_0_0_TRO_DF</t>
+  </si>
+  <si>
+    <t>PS_LPF_10-31_0_0_TRO_FS</t>
+  </si>
+  <si>
+    <t>PS_LPF_32-69_0_0_TRO_AF</t>
+  </si>
+  <si>
+    <t>PS_LPF_32-69_0_0_TRO_DF</t>
+  </si>
+  <si>
+    <t>PS_LPF_32-69_0_0_TRO_FS</t>
+  </si>
+  <si>
+    <t>PS_LPF_70-119_0_0_TRO_AF</t>
+  </si>
+  <si>
+    <t>PS_LPF_70-119_0_0_TRO_DF</t>
+  </si>
+  <si>
+    <t>PS_LPF_70-119_0_0_TRO_FS</t>
+  </si>
+  <si>
+    <t>Bluefin tuna (Thunnus thynnus) + Optional information about the School type/FADs</t>
+  </si>
+  <si>
+    <t>Albacore tuna (Thunnus alalunga) + Optional information about the School type/FADs</t>
+  </si>
+  <si>
+    <t>Skipjack tuna (Katsuwonus pelamis) Bigeye tuna (Thunnus obesus) Yellowfin tuna (Thunnus albacares) Albacore tuna (Thunnus alalunga) Bluefin tuna (Thunnus thynnus + Optional information about the School type/FADs</t>
+  </si>
+  <si>
+    <t>Swordfish (Xiphias gladius) + Optional information about the School type/FADs</t>
+  </si>
+  <si>
+    <t>Skipjack tuna (Katsuwonus pelamis) Yellowfin tuna (Thunnus albacares) Bigeye tuna (Thunnus obesus) + Optional information about the School type/FADs</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>Fishing on schools associated with anchored floating objects</t>
+  </si>
+  <si>
+    <t>DF</t>
+  </si>
+  <si>
+    <t>Fishing on schools associated with drifting floating objects</t>
+  </si>
+  <si>
+    <t>FS</t>
+  </si>
+  <si>
+    <t>Fishing on free schools (unassociated with floating objects)</t>
+  </si>
+  <si>
+    <t>Unknown (not specified)</t>
+  </si>
+  <si>
+    <t>Fishing mode (School type/FADs) codification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -232,8 +415,24 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -282,8 +481,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -291,11 +496,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -321,6 +610,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,19 +934,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="49.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="163.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1311,22 +1611,22 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="17" t="s">
+      <c r="B34" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="17" t="s">
+      <c r="C34" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E34" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34">
         <v>20240311</v>
       </c>
     </row>
@@ -1570,9 +1870,1005 @@
         <v>20230127</v>
       </c>
     </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E47" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="F47" s="17">
+        <v>20250130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F48" s="17">
+        <v>20250130</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F49" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F50" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F51" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F52" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F53" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F54" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F55" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E56" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F56" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F57" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E58" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F58" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D59" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E59" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F59" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B60" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D60" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E60" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="F60" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B61" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C61" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E61" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F61" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E62" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F62" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D63" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E63" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F63" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C64" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D64" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F64" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B65" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F65" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B66" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F66" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B67" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D67" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E67" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F67" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C68" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D68" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E68" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F68" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="C69" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E69" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F69" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C70" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E70" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F70" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B71" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C71" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D71" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E71" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F71" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="C72" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E72" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="F72" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D73" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E73" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F73" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B74" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C74" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D74" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E74" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F74" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C75" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D75" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E75" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="F75" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="C76" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D76" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E76" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F76" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B77" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="C77" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D77" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E77" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F77" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B78" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="C78" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D78" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E78" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F78" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C79" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D79" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F79" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B80" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C80" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D80" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E80" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F80" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B81" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C81" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D81" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F81" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C82" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D82" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F82" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C83" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D83" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F83" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C84" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D84" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F84" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B85" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D85" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F85" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B86" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C86" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D86" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E86" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F86" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B87" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="C87" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D87" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E87" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F87" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B88" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="C88" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D88" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F88" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B89" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="C89" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D89" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E89" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F89" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B90" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C90" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D90" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E90" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F90" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B91" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="C91" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D91" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E91" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F91" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B92" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="C92" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D92" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E92" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F92" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B93" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="C93" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D93" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E93" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="F93" s="17">
+        <v>20250110</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F46"/>
+  <autoFilter ref="A1:F46" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D4B456-9CED-46F7-80B2-919776CEB6BE}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="20"/>
+    </row>
+    <row r="2" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="25"/>
+      <c r="B6" s="26" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>